<commit_message>
Computing correlation for E2 quit rate x loc
</commit_message>
<xml_diff>
--- a/analysis/descriptive/Summary_descriptive.xlsx
+++ b/analysis/descriptive/Summary_descriptive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\ML_FaultUnderstanding\analysis\descriptive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A414AE3C-0771-4510-80C5-C713627A5958}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69795CCB-9B60-407A-A565-BBEE1DBD2B11}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18240" windowHeight="10996" activeTab="2" xr2:uid="{ABDA7A12-AE05-4412-AF9C-37CFA02479A8}"/>
   </bookViews>
@@ -23,10 +23,6 @@
     <sheet name="Language" sheetId="6" r:id="rId8"/>
     <sheet name="Summary" sheetId="7" r:id="rId9"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">TasksPerParticipant!$C$3:$C$11</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">TasksPerParticipant!$C$3:$C$11</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="134">
   <si>
     <t>E1</t>
   </si>
@@ -414,6 +410,39 @@
   </si>
   <si>
     <t>Correl removed outliers</t>
+  </si>
+  <si>
+    <t>Bug file</t>
+  </si>
+  <si>
+    <t>HIT02_24</t>
+  </si>
+  <si>
+    <t>HIT05_35</t>
+  </si>
+  <si>
+    <t>HIT01_8</t>
+  </si>
+  <si>
+    <t>HIT03_6</t>
+  </si>
+  <si>
+    <t>HIT06_51</t>
+  </si>
+  <si>
+    <t>HIT07_33</t>
+  </si>
+  <si>
+    <t>HIT08_54</t>
+  </si>
+  <si>
+    <t>HIT04_7</t>
+  </si>
+  <si>
+    <t>loc_E2</t>
+  </si>
+  <si>
+    <t>loc_E1</t>
   </si>
 </sst>
 </file>
@@ -518,7 +547,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -556,6 +585,9 @@
     <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2178,6 +2210,655 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200"/>
+              <a:t>Quit rate by size of methods (loc) for E1 and E2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14335892388451443"/>
+          <c:y val="0.17171296296296296"/>
+          <c:w val="0.82097440944881894"/>
+          <c:h val="0.62271617089530473"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TasksPerParticipant!$D$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TasksPerParticipant!$C$36:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TasksPerParticipant!$D$36:$D$43</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-473A-4B18-8BEB-0675633B6906}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TasksPerParticipant!$F$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>E1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TasksPerParticipant!$E$36:$E$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TasksPerParticipant!$F$36:$F$44</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.18404118404118405</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5637065637065631E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2175032175032175E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3166023166023165E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4157014157014158E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4157014157014158E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1583011583011582E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4157014157014158E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4157014157014158E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-473A-4B18-8BEB-0675633B6906}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="366584656"/>
+        <c:axId val="271654688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="366584656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Method size (loc)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="271654688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="271654688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Quite rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="366584656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.88932895888013996"/>
+          <c:y val="2.8564085739282562E-2"/>
+          <c:w val="6.9004374453193351E-2"/>
+          <c:h val="0.15625109361329836"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2264,6 +2945,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3297,6 +4018,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3919,6 +5156,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>488155</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>469105</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>88106</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFE7A5B8-7181-4736-9AC3-AC1F04582612}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5025,10 +6298,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982096B0-34AE-4D85-9C43-33DA390C3F2A}">
-  <dimension ref="B1:K12"/>
+  <dimension ref="B1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -5120,15 +6393,15 @@
         <v>6</v>
       </c>
       <c r="F4" t="str">
-        <f>D5</f>
+        <f t="shared" ref="F4:F11" si="0">D5</f>
         <v>1buggy_ApacheCamel.txt</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G11" si="0">E5</f>
+        <f t="shared" ref="G4:G11" si="1">E5</f>
         <v>62</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" ref="H4:H11" si="1">C4/777</f>
+        <f t="shared" ref="H4:H11" si="2">C4/777</f>
         <v>6.5637065637065631E-2</v>
       </c>
     </row>
@@ -5146,15 +6419,15 @@
         <v>62</v>
       </c>
       <c r="F5" t="str">
-        <f>D6</f>
+        <f t="shared" si="0"/>
         <v>9buggy_Hystrix_buggy.txt</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2175032175032175E-2</v>
       </c>
       <c r="J5" t="s">
@@ -5175,15 +6448,15 @@
         <v>2</v>
       </c>
       <c r="F6" t="str">
-        <f>D7</f>
+        <f t="shared" si="0"/>
         <v>13buggy_VectorClock_buggy.txt</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.3166023166023165E-2</v>
       </c>
     </row>
@@ -5201,15 +6474,15 @@
         <v>19</v>
       </c>
       <c r="F7" t="str">
-        <f>D8</f>
+        <f t="shared" si="0"/>
         <v>10HashPropertyBuilder_buggy.java</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4157014157014158E-2</v>
       </c>
     </row>
@@ -5227,15 +6500,15 @@
         <v>8</v>
       </c>
       <c r="F8" t="str">
-        <f>D9</f>
+        <f t="shared" si="0"/>
         <v>3buggy_PatchSetContentRemoteFactory_buggy.txt</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4157014157014158E-2</v>
       </c>
     </row>
@@ -5253,15 +6526,15 @@
         <v>34</v>
       </c>
       <c r="F9" t="str">
-        <f>D10</f>
+        <f t="shared" si="0"/>
         <v>7buggy_ReviewTaskMapper_buggy.txt</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1583011583011582E-2</v>
       </c>
     </row>
@@ -5279,15 +6552,15 @@
         <v>7</v>
       </c>
       <c r="F10" t="str">
-        <f>D11</f>
+        <f t="shared" si="0"/>
         <v>6ReviewScopeNode_buggy.java</v>
       </c>
       <c r="G10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4157014157014158E-2</v>
       </c>
     </row>
@@ -5305,15 +6578,15 @@
         <v>6</v>
       </c>
       <c r="F11" t="str">
-        <f>D12</f>
+        <f t="shared" si="0"/>
         <v>2SelectTranslator_buggy.java</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4157014157014158E-2</v>
       </c>
     </row>
@@ -5329,6 +6602,178 @@
       </c>
       <c r="E12">
         <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>119</v>
+      </c>
+      <c r="F34" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>133</v>
+      </c>
+      <c r="F35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="E36" s="24">
+        <v>6</v>
+      </c>
+      <c r="F36" s="4">
+        <v>0.18404118404118405</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37">
+        <v>7</v>
+      </c>
+      <c r="D37" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="E37" s="23">
+        <v>62</v>
+      </c>
+      <c r="F37" s="4">
+        <v>6.5637065637065631E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38">
+        <v>23</v>
+      </c>
+      <c r="D38" s="25">
+        <v>0.09</v>
+      </c>
+      <c r="E38" s="24">
+        <v>2</v>
+      </c>
+      <c r="F38" s="4">
+        <v>3.2175032175032175E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B39" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39">
+        <v>23</v>
+      </c>
+      <c r="D39" s="25">
+        <v>0.11</v>
+      </c>
+      <c r="E39" s="23">
+        <v>19</v>
+      </c>
+      <c r="F39" s="4">
+        <v>2.3166023166023165E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40">
+        <v>28</v>
+      </c>
+      <c r="D40" s="25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E40" s="24">
+        <v>8</v>
+      </c>
+      <c r="F40" s="4">
+        <v>1.4157014157014158E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41">
+        <v>12</v>
+      </c>
+      <c r="D41" s="25">
+        <v>0.06</v>
+      </c>
+      <c r="E41" s="23">
+        <v>34</v>
+      </c>
+      <c r="F41" s="4">
+        <v>1.4157014157014158E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B42" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42">
+        <v>33</v>
+      </c>
+      <c r="D42" s="25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E42" s="24">
+        <v>7</v>
+      </c>
+      <c r="F42" s="4">
+        <v>1.1583011583011582E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43">
+        <v>78</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0.15</v>
+      </c>
+      <c r="E43" s="23">
+        <v>6</v>
+      </c>
+      <c r="F43" s="4">
+        <v>1.4157014157014158E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="E44" s="24">
+        <v>41</v>
+      </c>
+      <c r="F44" s="4">
+        <v>1.4157014157014158E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New table about tasks left after quitting
</commit_message>
<xml_diff>
--- a/analysis/descriptive/Summary_descriptive.xlsx
+++ b/analysis/descriptive/Summary_descriptive.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\ML_FaultUnderstanding\analysis\descriptive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69795CCB-9B60-407A-A565-BBEE1DBD2B11}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BD3C5E-75A4-4BB0-B3DE-C13C405D954A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="18240" windowHeight="10996" activeTab="2" xr2:uid="{ABDA7A12-AE05-4412-AF9C-37CFA02479A8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="18278" windowHeight="10996" activeTab="2" xr2:uid="{ABDA7A12-AE05-4412-AF9C-37CFA02479A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="142">
   <si>
     <t>E1</t>
   </si>
@@ -443,13 +443,37 @@
   </si>
   <si>
     <t>loc_E1</t>
+  </si>
+  <si>
+    <t>Completed tasks in assignments</t>
+  </si>
+  <si>
+    <t>Number of assignments</t>
+  </si>
+  <si>
+    <t>Incomplete tasks</t>
+  </si>
+  <si>
+    <t>Incomplete rate</t>
+  </si>
+  <si>
+    <t>E2 incomplete tasks</t>
+  </si>
+  <si>
+    <t>E1 incomplete tasks</t>
+  </si>
+  <si>
+    <t>Completed tasks</t>
+  </si>
+  <si>
+    <t>Completed Tasks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,8 +505,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -507,8 +539,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -542,12 +580,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -588,12 +646,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5201,7 +5368,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{780B7287-B871-44B4-A107-C0E0AB69D85C}" name="Table2" displayName="Table2" ref="A37:E43" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{780B7287-B871-44B4-A107-C0E0AB69D85C}" name="Table2" displayName="Table2" ref="A37:E43" totalsRowShown="0" headerRowDxfId="21">
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A38:E42">
     <sortCondition ref="D37:D42"/>
   </sortState>
@@ -5209,10 +5376,10 @@
     <tableColumn id="1" xr3:uid="{1B853949-2C17-455A-8C99-7FF5A9859127}" name="Profession "/>
     <tableColumn id="2" xr3:uid="{4B3DD5EA-5764-4888-BFBA-20FCFF002CE3}" name="incomplete sessions"/>
     <tableColumn id="3" xr3:uid="{9C51F61A-03EA-4ABE-80EE-02B7AD30259A}" name="total sessions"/>
-    <tableColumn id="4" xr3:uid="{890C9E97-5763-4E3A-A061-F0726CFDEF84}" name="quit _x000a_rate" dataDxfId="8" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{890C9E97-5763-4E3A-A061-F0726CFDEF84}" name="quit _x000a_rate" dataDxfId="20" dataCellStyle="Percent">
       <calculatedColumnFormula>B38/C38</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{AA4CD94A-C1AC-43CA-9CBE-6C6CFE2A4091}" name="average incomplete tasks" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{AA4CD94A-C1AC-43CA-9CBE-6C6CFE2A4091}" name="average incomplete tasks" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5224,11 +5391,11 @@
     <tableColumn id="1" xr3:uid="{8589FE61-9738-45B0-B287-1EFCE741015B}" name="Score (# questions correct)"/>
     <tableColumn id="2" xr3:uid="{F814016F-721E-449D-AC2A-908A752B0774}" name="incomplete sessions"/>
     <tableColumn id="3" xr3:uid="{BE448F7C-4021-4ACC-91E5-5C0F3089EDA4}" name="total sessions"/>
-    <tableColumn id="4" xr3:uid="{00989F16-3776-453E-B7BF-C835415E558A}" name="quit rate" dataDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{00989F16-3776-453E-B7BF-C835415E558A}" name="quit rate" dataDxfId="18" dataCellStyle="Percent">
       <calculatedColumnFormula>B20/C20</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{E86217C2-5AC9-4E1A-9F16-6D9ECB3A2884}" name="average incomplete tasks"/>
-    <tableColumn id="6" xr3:uid="{5021B563-8E3D-4247-AE47-4FEFDDD62621}" name="% average incomplete tasks" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{5021B563-8E3D-4247-AE47-4FEFDDD62621}" name="% average incomplete tasks" dataDxfId="17">
       <calculatedColumnFormula>Table3[[#This Row],[average incomplete tasks]]/10</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5242,11 +5409,11 @@
     <tableColumn id="1" xr3:uid="{7F75C8DD-5FCF-4983-916C-F64811C2BBB0}" name="Score (# questions correct)"/>
     <tableColumn id="2" xr3:uid="{40AD7084-2ABB-45DB-8920-524649B2FBE3}" name="incomplete sessions"/>
     <tableColumn id="3" xr3:uid="{81F54010-81C4-48CA-B1F2-9B772C2F38E4}" name="total sessions"/>
-    <tableColumn id="4" xr3:uid="{F07CF7A7-024A-498F-9E2A-B7C039517C25}" name="quit rate" dataDxfId="4" dataCellStyle="Percent">
+    <tableColumn id="4" xr3:uid="{F07CF7A7-024A-498F-9E2A-B7C039517C25}" name="quit rate" dataDxfId="16" dataCellStyle="Percent">
       <calculatedColumnFormula>B26/C26</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0083674C-EDDC-43A1-8586-F423D35F21DD}" name="average incomplete tasks" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{DDB56D05-0DF6-4820-ABAC-44C9E4939CCE}" name="% average incomplete tasks" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="5" xr3:uid="{0083674C-EDDC-43A1-8586-F423D35F21DD}" name="average incomplete tasks" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{DDB56D05-0DF6-4820-ABAC-44C9E4939CCE}" name="% average incomplete tasks" dataDxfId="14" dataCellStyle="Percent">
       <calculatedColumnFormula>Table4[[#This Row],[average incomplete tasks]]/3</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{E088BD63-FE5E-4A57-A25D-C9A7F2D09F23}" name="Professionals"/>
@@ -5264,17 +5431,50 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{656F7524-5600-45F7-BCBB-BD055D7A195D}" name="Tasks"/>
     <tableColumn id="2" xr3:uid="{6BDA38FE-1455-422A-8E27-283AA156F2B4}" name="participants"/>
-    <tableColumn id="3" xr3:uid="{183C35EC-B221-4439-AAAA-CBC9A543698F}" name="Task order" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{183C35EC-B221-4439-AAAA-CBC9A543698F}" name="Task order" dataDxfId="13"/>
     <tableColumn id="4" xr3:uid="{B9C2667E-390C-4509-B795-0651887B8E89}" name="loc"/>
     <tableColumn id="5" xr3:uid="{C9AD113B-C9AE-435B-8273-D2DB79149774}" name="Quit at"/>
     <tableColumn id="6" xr3:uid="{618ECA55-3251-4A4C-8C03-56EB8BF74DD2}" name="loc2"/>
-    <tableColumn id="7" xr3:uid="{260DE00D-19E0-4C40-AF7D-3A59FFBE77E8}" name="Quit rate" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="7" xr3:uid="{260DE00D-19E0-4C40-AF7D-3A59FFBE77E8}" name="Quit rate" dataDxfId="12" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{33884AF4-0ADF-4DC6-8F7A-50A0C0A9616F}" name="Table6" displayName="Table6" ref="B50:F54" totalsRowShown="0" headerRowDxfId="11">
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D8436B48-8864-4716-B975-7522006FD6A0}" name="Completed tasks in assignments"/>
+    <tableColumn id="2" xr3:uid="{D5A8169E-C524-4030-880B-2511BCDA580D}" name="Number of assignments"/>
+    <tableColumn id="3" xr3:uid="{23C1ABA4-A5DE-4394-95CF-66F25CD3CEFF}" name="Completed Tasks"/>
+    <tableColumn id="4" xr3:uid="{913EBB25-28F6-416E-B3E9-031A88F9102C}" name="Incomplete tasks" dataDxfId="10">
+      <calculatedColumnFormula>(3-Table6[[#This Row],[Completed tasks in assignments]])*Table6[[#This Row],[Number of assignments]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{91C538DA-9438-414B-8050-1819F3C81507}" name="Incomplete rate" dataDxfId="9">
+      <calculatedColumnFormula>Table6[[#This Row],[Incomplete tasks]]/(Table6[[#This Row],[Completed Tasks]]+Table6[[#This Row],[Incomplete tasks]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8A29C771-8E74-402D-9A8B-07D2014DAD6F}" name="Table7" displayName="Table7" ref="B57:F67" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
+  <autoFilter ref="B57:F67" xr:uid="{B1571A41-CDAA-4E45-BD9A-2E860F66C242}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{9EA52DC6-5CAA-4B6E-AF58-A84E3C65AD1A}" name="Completed tasks in assignments" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{BD8547E9-128A-40A7-AD9B-393732E36DD9}" name="Number of assignments" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{45A17975-7691-4970-9EE6-FEDEA7E9F50C}" name="Completed tasks" dataDxfId="4">
+      <calculatedColumnFormula>C58*B58</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{31D09BE0-F531-4A32-A7C3-F3A266F25F5A}" name="Incomplete tasks" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{2BA77099-DD7E-4C62-BEA7-B658F93235AC}" name="Incomplete rate" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4124DC2-372B-4D32-B7EF-2AB8C9CEF9AF}" name="Table1" displayName="Table1" ref="B1:D17" totalsRowShown="0">
   <autoFilter ref="B1:D17" xr:uid="{7B066246-CBDD-4621-B81C-79B9EC096175}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C12">
@@ -6298,16 +6498,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982096B0-34AE-4D85-9C43-33DA390C3F2A}">
-  <dimension ref="B1:K44"/>
+  <dimension ref="B1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="12.19921875" customWidth="1"/>
-    <col min="4" max="4" width="11.1328125" customWidth="1"/>
+    <col min="2" max="2" width="18.46484375" customWidth="1"/>
+    <col min="3" max="3" width="13.73046875" customWidth="1"/>
+    <col min="4" max="4" width="11.265625" customWidth="1"/>
+    <col min="5" max="5" width="10.73046875" customWidth="1"/>
+    <col min="6" max="6" width="10.86328125" customWidth="1"/>
     <col min="8" max="8" width="9.86328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6776,12 +6979,335 @@
         <v>1.4157014157014158E-2</v>
       </c>
     </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B49" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="31.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B50" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>45</v>
+      </c>
+      <c r="D51">
+        <f>C51*B51</f>
+        <v>45</v>
+      </c>
+      <c r="E51">
+        <f>(3-Table6[[#This Row],[Completed tasks in assignments]])*Table6[[#This Row],[Number of assignments]]</f>
+        <v>90</v>
+      </c>
+      <c r="F51" s="4">
+        <f>Table6[[#This Row],[Incomplete tasks]]/(Table6[[#This Row],[Completed Tasks]]+Table6[[#This Row],[Incomplete tasks]])</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>123</v>
+      </c>
+      <c r="D52">
+        <f t="shared" ref="D52:D53" si="3">C52*B52</f>
+        <v>246</v>
+      </c>
+      <c r="E52">
+        <f>(3-Table6[[#This Row],[Completed tasks in assignments]])*Table6[[#This Row],[Number of assignments]]</f>
+        <v>123</v>
+      </c>
+      <c r="F52" s="4">
+        <f>Table6[[#This Row],[Incomplete tasks]]/(Table6[[#This Row],[Completed Tasks]]+Table6[[#This Row],[Incomplete tasks]])</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>763</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="3"/>
+        <v>2289</v>
+      </c>
+      <c r="E53">
+        <f>(3-Table6[[#This Row],[Completed tasks in assignments]])*Table6[[#This Row],[Number of assignments]]</f>
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <f>Table6[[#This Row],[Incomplete tasks]]/(Table6[[#This Row],[Completed Tasks]]+Table6[[#This Row],[Incomplete tasks]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="5">
+        <f>SUM(D51:D53)</f>
+        <v>2580</v>
+      </c>
+      <c r="E54">
+        <f>SUM(E51:E53)</f>
+        <v>213</v>
+      </c>
+      <c r="F54" s="31">
+        <f>Table6[[#This Row],[Incomplete tasks]]/Table6[[#This Row],[Completed Tasks]]</f>
+        <v>8.2558139534883723E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B56" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B57" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C57" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="E57" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="F57" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B58" s="29">
+        <v>1</v>
+      </c>
+      <c r="C58" s="29">
+        <v>143</v>
+      </c>
+      <c r="D58" s="30">
+        <f>C58*B58</f>
+        <v>143</v>
+      </c>
+      <c r="E58" s="30">
+        <f>(10-B58)*C58</f>
+        <v>1287</v>
+      </c>
+      <c r="F58" s="30">
+        <f>E58/(D58+E58)</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B59" s="29">
+        <v>2</v>
+      </c>
+      <c r="C59" s="29">
+        <v>51</v>
+      </c>
+      <c r="D59" s="30">
+        <f t="shared" ref="D59:D67" si="4">C59*B59</f>
+        <v>102</v>
+      </c>
+      <c r="E59" s="30">
+        <f t="shared" ref="E59:E67" si="5">(10-B59)*C59</f>
+        <v>408</v>
+      </c>
+      <c r="F59" s="30">
+        <f t="shared" ref="F59:F67" si="6">E59/(D59+E59)</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B60" s="29">
+        <v>3</v>
+      </c>
+      <c r="C60" s="29">
+        <v>25</v>
+      </c>
+      <c r="D60" s="30">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="E60" s="30">
+        <f t="shared" si="5"/>
+        <v>175</v>
+      </c>
+      <c r="F60" s="30">
+        <f t="shared" si="6"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B61" s="29">
+        <v>4</v>
+      </c>
+      <c r="C61" s="29">
+        <v>18</v>
+      </c>
+      <c r="D61" s="30">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="E61" s="30">
+        <f t="shared" si="5"/>
+        <v>108</v>
+      </c>
+      <c r="F61" s="30">
+        <f t="shared" si="6"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B62" s="29">
+        <v>5</v>
+      </c>
+      <c r="C62" s="29">
+        <v>11</v>
+      </c>
+      <c r="D62" s="30">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="E62" s="30">
+        <f t="shared" si="5"/>
+        <v>55</v>
+      </c>
+      <c r="F62" s="30">
+        <f t="shared" si="6"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B63" s="29">
+        <v>6</v>
+      </c>
+      <c r="C63" s="29">
+        <v>11</v>
+      </c>
+      <c r="D63" s="30">
+        <f t="shared" si="4"/>
+        <v>66</v>
+      </c>
+      <c r="E63" s="30">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+      <c r="F63" s="30">
+        <f t="shared" si="6"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B64" s="29">
+        <v>7</v>
+      </c>
+      <c r="C64" s="29">
+        <v>9</v>
+      </c>
+      <c r="D64" s="30">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="E64" s="30">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="F64" s="30">
+        <f t="shared" si="6"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B65" s="29">
+        <v>8</v>
+      </c>
+      <c r="C65" s="29">
+        <v>11</v>
+      </c>
+      <c r="D65" s="30">
+        <f t="shared" si="4"/>
+        <v>88</v>
+      </c>
+      <c r="E65" s="30">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="F65" s="30">
+        <f t="shared" si="6"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B66" s="29">
+        <v>9</v>
+      </c>
+      <c r="C66" s="29">
+        <v>11</v>
+      </c>
+      <c r="D66" s="30">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="E66" s="30">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="F66" s="30">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B67" s="26">
+        <v>10</v>
+      </c>
+      <c r="C67" s="26">
+        <v>487</v>
+      </c>
+      <c r="D67" s="30">
+        <f t="shared" si="4"/>
+        <v>4870</v>
+      </c>
+      <c r="E67" s="30">
+        <f>SUM(E58:E66)</f>
+        <v>2137</v>
+      </c>
+      <c r="F67" s="31">
+        <f>E67/D67</f>
+        <v>0.43880903490759754</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Created a new table for quit rate and computed correlations
</commit_message>
<xml_diff>
--- a/analysis/descriptive/Summary_descriptive.xlsx
+++ b/analysis/descriptive/Summary_descriptive.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\ML_FaultUnderstanding\analysis\descriptive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BD3C5E-75A4-4BB0-B3DE-C13C405D954A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4110ED-AB1D-4185-8DE2-43035D73AD32}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18278" windowHeight="10996" activeTab="2" xr2:uid="{ABDA7A12-AE05-4412-AF9C-37CFA02479A8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
   <si>
     <t>E1</t>
   </si>
@@ -467,6 +467,12 @@
   </si>
   <si>
     <t>Completed Tasks</t>
+  </si>
+  <si>
+    <t>incomplete</t>
+  </si>
+  <si>
+    <t>CONFIRM THAT THESE NUMBERS ARE CORRECT</t>
   </si>
 </sst>
 </file>
@@ -546,7 +552,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -600,12 +606,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -656,45 +742,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -737,13 +801,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </left>
@@ -751,6 +808,46 @@
           <color theme="4" tint="0.39997558519241921"/>
         </top>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2688,6 +2785,115 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TasksPerParticipant!$H$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>quit rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TasksPerParticipant!$C$36:$C$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TasksPerParticipant!$H$36:$H$43</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.45205479452054698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29166666666666602</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19626168224299001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.214285714285714</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.1743119266054995E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0975609756097497E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.245283018867924</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.125925925925925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-833F-4C47-AAB1-8B1FF626F91E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2949,8 +3155,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.88932895888013996"/>
           <c:y val="2.8564085739282562E-2"/>
-          <c:w val="6.9004374453193351E-2"/>
-          <c:h val="0.15625109361329836"/>
+          <c:w val="0.11067104111986002"/>
+          <c:h val="0.23356564858458437"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -5330,16 +5536,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>488155</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>73817</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>59531</xdr:rowOff>
+      <xdr:rowOff>78581</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>469105</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>111917</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>88106</xdr:rowOff>
+      <xdr:rowOff>107156</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5459,16 +5665,16 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8A29C771-8E74-402D-9A8B-07D2014DAD6F}" name="Table7" displayName="Table7" ref="B57:F67" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="7" tableBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8A29C771-8E74-402D-9A8B-07D2014DAD6F}" name="Table7" displayName="Table7" ref="B57:F67" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5">
   <autoFilter ref="B57:F67" xr:uid="{B1571A41-CDAA-4E45-BD9A-2E860F66C242}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9EA52DC6-5CAA-4B6E-AF58-A84E3C65AD1A}" name="Completed tasks in assignments" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{BD8547E9-128A-40A7-AD9B-393732E36DD9}" name="Number of assignments" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{45A17975-7691-4970-9EE6-FEDEA7E9F50C}" name="Completed tasks" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{9EA52DC6-5CAA-4B6E-AF58-A84E3C65AD1A}" name="Completed tasks in assignments" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{BD8547E9-128A-40A7-AD9B-393732E36DD9}" name="Number of assignments" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{45A17975-7691-4970-9EE6-FEDEA7E9F50C}" name="Completed tasks" dataDxfId="2">
       <calculatedColumnFormula>C58*B58</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{31D09BE0-F531-4A32-A7C3-F3A266F25F5A}" name="Incomplete tasks" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{2BA77099-DD7E-4C62-BEA7-B658F93235AC}" name="Incomplete rate" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{31D09BE0-F531-4A32-A7C3-F3A266F25F5A}" name="Incomplete tasks" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{2BA77099-DD7E-4C62-BEA7-B658F93235AC}" name="Incomplete rate" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5924,8 +6130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81D6450-D6F5-4F69-8BE3-C113B4477E1F}">
   <dimension ref="A2:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:E43"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6500,8 +6706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982096B0-34AE-4D85-9C43-33DA390C3F2A}">
   <dimension ref="B1:K67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6807,7 +7013,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B34" t="s">
         <v>1</v>
       </c>
@@ -6817,8 +7023,11 @@
       <c r="F34" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G34" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
         <v>123</v>
       </c>
@@ -6834,8 +7043,18 @@
       <c r="F35" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G35" s="32"/>
+      <c r="H35" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="J35" s="34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>124</v>
       </c>
@@ -6851,8 +7070,20 @@
       <c r="F36" s="4">
         <v>0.18404118404118405</v>
       </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G36" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="H36" s="36">
+        <v>0.45205479452054698</v>
+      </c>
+      <c r="I36" s="37">
+        <v>73</v>
+      </c>
+      <c r="J36" s="38">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>125</v>
       </c>
@@ -6868,8 +7099,20 @@
       <c r="F37" s="4">
         <v>6.5637065637065631E-2</v>
       </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G37" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="H37" s="36">
+        <v>0.29166666666666602</v>
+      </c>
+      <c r="I37" s="37">
+        <v>24</v>
+      </c>
+      <c r="J37" s="38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>126</v>
       </c>
@@ -6885,8 +7128,20 @@
       <c r="F38" s="4">
         <v>3.2175032175032175E-2</v>
       </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G38" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="H38" s="36">
+        <v>0.19626168224299001</v>
+      </c>
+      <c r="I38" s="37">
+        <v>107</v>
+      </c>
+      <c r="J38" s="38">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B39" t="s">
         <v>127</v>
       </c>
@@ -6902,8 +7157,20 @@
       <c r="F39" s="4">
         <v>2.3166023166023165E-2</v>
       </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G39" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="H39" s="36">
+        <v>0.214285714285714</v>
+      </c>
+      <c r="I39" s="37">
+        <v>266</v>
+      </c>
+      <c r="J39" s="38">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>128</v>
       </c>
@@ -6919,8 +7186,20 @@
       <c r="F40" s="4">
         <v>1.4157014157014158E-2</v>
       </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G40" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="H40" s="36">
+        <v>9.1743119266054995E-2</v>
+      </c>
+      <c r="I40" s="37">
+        <v>109</v>
+      </c>
+      <c r="J40" s="38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B41" t="s">
         <v>129</v>
       </c>
@@ -6936,8 +7215,20 @@
       <c r="F41" s="4">
         <v>1.4157014157014158E-2</v>
       </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G41" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" s="36">
+        <v>6.0975609756097497E-2</v>
+      </c>
+      <c r="I41" s="37">
+        <v>164</v>
+      </c>
+      <c r="J41" s="38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>130</v>
       </c>
@@ -6953,8 +7244,20 @@
       <c r="F42" s="4">
         <v>1.1583011583011582E-2</v>
       </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G42" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="H42" s="36">
+        <v>0.245283018867924</v>
+      </c>
+      <c r="I42" s="37">
+        <v>53</v>
+      </c>
+      <c r="J42" s="38">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
         <v>131</v>
       </c>
@@ -6970,13 +7273,50 @@
       <c r="F43" s="4">
         <v>1.4157014157014158E-2</v>
       </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="G43" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="H43" s="36">
+        <v>0.125925925925925</v>
+      </c>
+      <c r="I43" s="37">
+        <v>135</v>
+      </c>
+      <c r="J43" s="38">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="E44" s="24">
         <v>41</v>
       </c>
       <c r="F44" s="4">
         <v>1.4157014157014158E-2</v>
+      </c>
+      <c r="G44" s="39"/>
+      <c r="H44" s="40">
+        <f>J44/I44</f>
+        <v>0.18045112781954886</v>
+      </c>
+      <c r="I44" s="41">
+        <f>SUM(I36:I43)</f>
+        <v>931</v>
+      </c>
+      <c r="J44" s="42">
+        <f>SUM(J36:J43)</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="G46">
+        <f>CORREL(H36:H43,C36:C43)</f>
+        <v>-0.45452813833369993</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="G47">
+        <f>CORREL(C36:C43,D36:D43)</f>
+        <v>0.8756663596482317</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.45">
@@ -7132,11 +7472,11 @@
         <v>102</v>
       </c>
       <c r="E59" s="30">
-        <f t="shared" ref="E59:E67" si="5">(10-B59)*C59</f>
+        <f t="shared" ref="E59:E66" si="5">(10-B59)*C59</f>
         <v>408</v>
       </c>
       <c r="F59" s="30">
-        <f t="shared" ref="F59:F67" si="6">E59/(D59+E59)</f>
+        <f t="shared" ref="F59:F66" si="6">E59/(D59+E59)</f>
         <v>0.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Summary of score frequencies E1 and E2
</commit_message>
<xml_diff>
--- a/analysis/descriptive/Summary_descriptive.xlsx
+++ b/analysis/descriptive/Summary_descriptive.xlsx
@@ -8,26 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\ML_FaultUnderstanding\analysis\descriptive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F2DB06-F5C9-4AA5-A2A8-7C4188178C81}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21E40C0-1647-4AA5-BB74-16B230061F03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="18278" windowHeight="10996" tabRatio="735" activeTab="7" xr2:uid="{ABDA7A12-AE05-4412-AF9C-37CFA02479A8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="18278" windowHeight="10996" tabRatio="735" firstSheet="2" activeTab="3" xr2:uid="{ABDA7A12-AE05-4412-AF9C-37CFA02479A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Gender" sheetId="1" r:id="rId1"/>
     <sheet name="Quit_Rate" sheetId="8" r:id="rId2"/>
     <sheet name="TasksPerParticipant" sheetId="9" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId4"/>
+    <sheet name="Score" sheetId="10" r:id="rId4"/>
     <sheet name="Country" sheetId="3" r:id="rId5"/>
     <sheet name="Age" sheetId="2" r:id="rId6"/>
     <sheet name="Professions" sheetId="4" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId8"/>
+    <sheet name="Gender by Profession" sheetId="11" r:id="rId8"/>
     <sheet name="YoE" sheetId="5" r:id="rId9"/>
     <sheet name="Language" sheetId="6" r:id="rId10"/>
     <sheet name="Summary" sheetId="7" r:id="rId11"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId12"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="209">
   <si>
     <t>E1</t>
   </si>
@@ -480,9 +477,6 @@
     <t>CONFIRM THAT THESE NUMBERS ARE CORRECT</t>
   </si>
   <si>
-    <t>G</t>
-  </si>
-  <si>
     <t>Female</t>
   </si>
   <si>
@@ -652,6 +646,30 @@
   </si>
   <si>
     <t>Are the frequencies of female and males distinct across professions? Chi-square test for that.</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>This shows that E2 qualification test spread participants more evenly across the three qualification levels.</t>
+  </si>
+  <si>
+    <t>The Chisquare test confirmed that that experiment assignment and the levels of qualification were independent.</t>
+  </si>
+  <si>
+    <t>We donfirmed that these proportion are distinct by running a chisquare test to evaluate the independence</t>
+  </si>
+  <si>
+    <t>between independent from the qualification score levels (chisquare 201,14, df=2, p-value&lt;0.0001)</t>
   </si>
 </sst>
 </file>
@@ -4230,7 +4248,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$5</c:f>
+              <c:f>'Gender by Profession'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4251,7 +4269,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$4:$F$4</c:f>
+              <c:f>'Gender by Profession'!$B$4:$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4274,7 +4292,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$5:$F$5</c:f>
+              <c:f>'Gender by Profession'!$B$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4307,7 +4325,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$6</c:f>
+              <c:f>'Gender by Profession'!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4328,7 +4346,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$4:$F$4</c:f>
+              <c:f>'Gender by Profession'!$B$4:$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4351,7 +4369,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$6:$F$6</c:f>
+              <c:f>'Gender by Profession'!$B$6:$F$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4384,7 +4402,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$7</c:f>
+              <c:f>'Gender by Profession'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4405,7 +4423,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$4:$F$4</c:f>
+              <c:f>'Gender by Profession'!$B$4:$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4428,7 +4446,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$7:$F$7</c:f>
+              <c:f>'Gender by Profession'!$B$7:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4461,7 +4479,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$8</c:f>
+              <c:f>'Gender by Profession'!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4482,7 +4500,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$4:$F$4</c:f>
+              <c:f>'Gender by Profession'!$B$4:$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4505,7 +4523,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$8:$F$8</c:f>
+              <c:f>'Gender by Profession'!$B$8:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4809,7 +4827,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$12</c:f>
+              <c:f>'Gender by Profession'!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4830,7 +4848,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$11:$F$11</c:f>
+              <c:f>'Gender by Profession'!$B$11:$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4853,7 +4871,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$12:$F$12</c:f>
+              <c:f>'Gender by Profession'!$B$12:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4886,7 +4904,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$13</c:f>
+              <c:f>'Gender by Profession'!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4907,7 +4925,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$11:$F$11</c:f>
+              <c:f>'Gender by Profession'!$B$11:$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -4930,7 +4948,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$13:$F$13</c:f>
+              <c:f>'Gender by Profession'!$B$13:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -4963,7 +4981,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$14</c:f>
+              <c:f>'Gender by Profession'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4984,7 +5002,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$11:$F$11</c:f>
+              <c:f>'Gender by Profession'!$B$11:$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -5007,7 +5025,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$14:$F$14</c:f>
+              <c:f>'Gender by Profession'!$B$14:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -5040,7 +5058,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$A$15</c:f>
+              <c:f>'Gender by Profession'!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5061,7 +5079,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$B$11:$F$11</c:f>
+              <c:f>'Gender by Profession'!$B$11:$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -5084,7 +5102,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$15:$F$15</c:f>
+              <c:f>'Gender by Profession'!$B$15:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -8815,75 +8833,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="gender_profession"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>Gender</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>Professional_Developer</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>Hobbyist</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>female</v>
-          </cell>
-          <cell r="B3">
-            <v>0.26035502958579798</v>
-          </cell>
-          <cell r="C3">
-            <v>0.25225225225225201</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>male</v>
-          </cell>
-          <cell r="B4">
-            <v>0.73964497041420096</v>
-          </cell>
-          <cell r="C4">
-            <v>0.74774774774774699</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>prefer not tell</v>
-          </cell>
-          <cell r="B5">
-            <v>0</v>
-          </cell>
-          <cell r="C5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>other</v>
-          </cell>
-          <cell r="B6">
-            <v>0</v>
-          </cell>
-          <cell r="C6">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{34CED1F8-1E6C-4A36-ABEE-5484A59D808D}" name="Table29" displayName="Table29" ref="B12:H16" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <tableColumns count="7">
@@ -8900,6 +8849,20 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6F75031B-11C3-49FA-B71C-EDC3763F37B2}" name="Table11" displayName="Table11" ref="A2:E5" totalsRowShown="0">
+  <autoFilter ref="A2:E5" xr:uid="{5E06F2C4-B735-47D1-B35B-A036D3232E4F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{797B4291-6E16-4214-AD26-96D635010F52}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{9CA10DBF-E249-47B5-8213-3F5E3AF122C5}" name="low"/>
+    <tableColumn id="3" xr3:uid="{E6C383A1-5859-4F6A-9E1C-A916817D7111}" name="medium"/>
+    <tableColumn id="4" xr3:uid="{3B85EDB2-57BC-4B32-828E-562B870623DD}" name="high"/>
+    <tableColumn id="5" xr3:uid="{653DBA1C-D1B1-4448-B717-13A5718FCE7D}" name="total"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C4124DC2-372B-4D32-B7EF-2AB8C9CEF9AF}" name="Table1" displayName="Table1" ref="B1:D17" totalsRowShown="0">
   <autoFilter ref="B1:D17" xr:uid="{7B066246-CBDD-4621-B81C-79B9EC096175}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C12">
@@ -9484,7 +9447,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B11" s="35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
@@ -9495,13 +9458,13 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B12" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="D12" s="37" t="s">
         <v>150</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>151</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>78</v>
@@ -9518,7 +9481,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B13" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C13" s="40">
         <v>30.0386740331491</v>
@@ -9541,7 +9504,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B14" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C14" s="40">
         <v>31.451127819548802</v>
@@ -9564,7 +9527,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B15" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C15" s="40">
         <v>1.5340055661737</v>
@@ -9587,7 +9550,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B16" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C16" s="43">
         <v>0.125028283434515</v>
@@ -9610,7 +9573,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B18" s="35" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
@@ -9621,13 +9584,13 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B19" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="D19" s="37" t="s">
         <v>150</v>
-      </c>
-      <c r="D19" s="37" t="s">
-        <v>151</v>
       </c>
       <c r="E19" s="37" t="s">
         <v>78</v>
@@ -9644,7 +9607,7 @@
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B20" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" s="45">
         <v>1.3026359818355E-15</v>
@@ -9667,7 +9630,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B21" s="42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C21" s="46">
         <v>7.36442551385607E-9</v>
@@ -9690,7 +9653,7 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B23" s="35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="35"/>
@@ -9701,13 +9664,13 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B24" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C24" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="D24" s="37" t="s">
         <v>150</v>
-      </c>
-      <c r="D24" s="37" t="s">
-        <v>151</v>
       </c>
       <c r="E24" s="37" t="s">
         <v>78</v>
@@ -9724,7 +9687,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B25" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C25" s="40">
         <v>28</v>
@@ -9747,7 +9710,7 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B26" s="42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C26" s="43">
         <v>30</v>
@@ -11612,21 +11575,161 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A945A360-833E-477D-9D02-BCB5EEFB1799}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="9.86328125" customWidth="1"/>
+    <col min="3" max="3" width="9.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>144</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>538</v>
+      </c>
+      <c r="C3">
+        <v>134</v>
+      </c>
+      <c r="D3">
+        <v>105</v>
+      </c>
+      <c r="E3">
+        <f>SUM(B3:D3)</f>
+        <v>777</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>146</v>
+      </c>
+      <c r="C4">
+        <v>157</v>
+      </c>
+      <c r="D4">
+        <v>194</v>
+      </c>
+      <c r="E4">
+        <f>SUM(B4:D4)</f>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>684</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:D5" si="0">SUM(C3:C4)</f>
+        <v>291</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C7" t="s">
+        <v>202</v>
+      </c>
+      <c r="D7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <f>B3/B5</f>
+        <v>0.78654970760233922</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:D8" si="1">C3/C5</f>
+        <v>0.46048109965635736</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.3511705685618729</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <f>B4/B5</f>
+        <v>0.21345029239766081</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:D9" si="2">C4/C5</f>
+        <v>0.53951890034364258</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>0.6488294314381271</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -11946,182 +12049,182 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B15" s="49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B16" s="49" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" s="49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" s="49" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" s="49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" s="49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B22" s="49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B23" s="49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B24" s="49" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B25" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B26" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B27" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B28" s="49" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B29" s="49" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B30" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B31" s="49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B32" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B34" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B35" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B36" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B37" s="49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B38" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B39" s="49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B40" s="49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B41" s="49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B42" s="49" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B43" s="49" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B44" s="49" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B45" s="49" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B46" s="49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B47" s="49" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B48" s="49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B49" s="49" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B50" s="50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -12134,7 +12237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A7A90A3-EF4D-468C-B579-EF7A4FC09F2E}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -12142,20 +12245,20 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
         <v>78</v>
@@ -12172,7 +12275,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B5">
         <v>0.26035502958579798</v>
@@ -12192,7 +12295,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6">
         <v>0.73964497041420096</v>
@@ -12212,7 +12315,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -12252,15 +12355,15 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
         <v>78</v>
@@ -12280,7 +12383,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B12">
         <v>44</v>
@@ -12304,7 +12407,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B13">
         <v>125</v>
@@ -12328,7 +12431,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -12376,7 +12479,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B16">
         <f>SUM(B12:B15)</f>
@@ -12405,26 +12508,26 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" t="s">
         <v>192</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>193</v>
       </c>
-      <c r="C20" t="s">
-        <v>194</v>
-      </c>
       <c r="D20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E20" t="s">
         <v>48</v>
@@ -12435,7 +12538,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B21">
         <v>254</v>

</xml_diff>